<commit_message>
targets and excretion analisis
</commit_message>
<xml_diff>
--- a/cuasinoides.xlsx
+++ b/cuasinoides.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="cuasinoides" sheetId="2" r:id="rId1"/>
@@ -12,10 +12,9 @@
     <sheet name="pkcsm" sheetId="5" r:id="rId3"/>
     <sheet name="swissadme" sheetId="4" r:id="rId4"/>
     <sheet name="act_biologic" sheetId="7" r:id="rId5"/>
-    <sheet name="Target" sheetId="8" r:id="rId6"/>
+    <sheet name="target" sheetId="8" r:id="rId6"/>
     <sheet name="protox" sheetId="9" r:id="rId7"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId8"/>
-    <sheet name="Hoja2" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4213" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4899" uniqueCount="867">
   <si>
     <t>Eurycoma longifolia </t>
   </si>
@@ -2261,68 +2260,470 @@
     <t>Solubilidad (mg/mL)</t>
   </si>
   <si>
-    <t>OCT2 Probability:</t>
-  </si>
-  <si>
-    <t>------------------------------</t>
-  </si>
-  <si>
-    <t>Clearance Predictions:</t>
-  </si>
-  <si>
-    <t>Half-Life Probability:</t>
-  </si>
-  <si>
-    <t>Mean:</t>
-  </si>
-  <si>
-    <t>Sample</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>(n):</t>
-  </si>
-  <si>
-    <t>Median:</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>deviation:</t>
-  </si>
-  <si>
-    <t>Minimum:</t>
-  </si>
-  <si>
-    <t>25th</t>
-  </si>
-  <si>
-    <t>percentile:</t>
-  </si>
-  <si>
-    <t>75th</t>
-  </si>
-  <si>
-    <t>Maximum:</t>
-  </si>
-  <si>
-    <t>IQR:</t>
-  </si>
-  <si>
-    <t>Missing</t>
-  </si>
-  <si>
-    <t>values:</t>
+    <t>0,914</t>
+  </si>
+  <si>
+    <t>0,005</t>
+  </si>
+  <si>
+    <t>Antineoplastic</t>
+  </si>
+  <si>
+    <t>0,732</t>
+  </si>
+  <si>
+    <t>0,013</t>
+  </si>
+  <si>
+    <t>Immunosuppressant</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>0,951</t>
+  </si>
+  <si>
+    <t>0,004</t>
+  </si>
+  <si>
+    <t>0,739</t>
+  </si>
+  <si>
+    <t>Antineoplastic (breast cancer)</t>
+  </si>
+  <si>
+    <t>0,712</t>
+  </si>
+  <si>
+    <t>Antineoplastic (lung cancer)</t>
+  </si>
+  <si>
+    <t>0,718</t>
+  </si>
+  <si>
+    <t>0,049</t>
+  </si>
+  <si>
+    <t>Testosterone 17beta-dehydrogenase (NADP+) inhibitor</t>
+  </si>
+  <si>
+    <t>0,707</t>
+  </si>
+  <si>
+    <t>0,043</t>
+  </si>
+  <si>
+    <t>Antieczematic</t>
+  </si>
+  <si>
+    <t>0,937</t>
+  </si>
+  <si>
+    <t>0,791</t>
+  </si>
+  <si>
+    <t>0,020</t>
+  </si>
+  <si>
+    <t>0,728</t>
+  </si>
+  <si>
+    <t>0,955</t>
+  </si>
+  <si>
+    <t>0,843</t>
+  </si>
+  <si>
+    <t>0,001</t>
+  </si>
+  <si>
+    <t>Polarisation stimulant</t>
+  </si>
+  <si>
+    <t>0,846</t>
+  </si>
+  <si>
+    <t>0,010</t>
+  </si>
+  <si>
+    <t>0,801</t>
+  </si>
+  <si>
+    <t>0,771</t>
+  </si>
+  <si>
+    <t>0,002</t>
+  </si>
+  <si>
+    <t>Myc inhibitor</t>
+  </si>
+  <si>
+    <t>0,777</t>
+  </si>
+  <si>
+    <t>0,009</t>
+  </si>
+  <si>
+    <t>Apoptosis agonist</t>
+  </si>
+  <si>
+    <t>0,772</t>
+  </si>
+  <si>
+    <t>0,008</t>
+  </si>
+  <si>
+    <t>Immunosuppressan</t>
+  </si>
+  <si>
+    <t>0,984</t>
+  </si>
+  <si>
+    <t>0,982</t>
+  </si>
+  <si>
+    <t>Antileukemic</t>
+  </si>
+  <si>
+    <t>0,977</t>
+  </si>
+  <si>
+    <t>0,000</t>
+  </si>
+  <si>
+    <t>0,953</t>
+  </si>
+  <si>
+    <t>Cytostatic</t>
+  </si>
+  <si>
+    <t>0,912</t>
+  </si>
+  <si>
+    <t>Antiprotozoal (Plasmodium)</t>
+  </si>
+  <si>
+    <t>0,894</t>
+  </si>
+  <si>
+    <t>Transcription factor inhibitor</t>
+  </si>
+  <si>
+    <t>0,896</t>
+  </si>
+  <si>
+    <t>0,864</t>
+  </si>
+  <si>
+    <t>0,828</t>
+  </si>
+  <si>
+    <t>Antineoplastic (multiple myeloma)</t>
+  </si>
+  <si>
+    <t>0,745</t>
+  </si>
+  <si>
+    <t>0,003</t>
+  </si>
+  <si>
+    <t>Antineoplastic (cervical cancer)</t>
+  </si>
+  <si>
+    <t>0,751</t>
+  </si>
+  <si>
+    <t>0,030</t>
+  </si>
+  <si>
+    <t>0,726</t>
+  </si>
+  <si>
+    <t>0,014</t>
+  </si>
+  <si>
+    <t>0,968</t>
+  </si>
+  <si>
+    <t>0,961</t>
+  </si>
+  <si>
+    <t>0,954</t>
+  </si>
+  <si>
+    <t>Hypoxia inducible factor 1 alpha inhibitor</t>
+  </si>
+  <si>
+    <t>0,947</t>
+  </si>
+  <si>
+    <t>0,900</t>
+  </si>
+  <si>
+    <t>0,877</t>
+  </si>
+  <si>
+    <t>CDP-glycerol glycerophosphotransferase inhibitor</t>
+  </si>
+  <si>
+    <t>0,832</t>
+  </si>
+  <si>
+    <t>0,006</t>
+  </si>
+  <si>
+    <t>0,978</t>
+  </si>
+  <si>
+    <t>0,962</t>
+  </si>
+  <si>
+    <t>0,904</t>
+  </si>
+  <si>
+    <t>0,837</t>
+  </si>
+  <si>
+    <t>0,821</t>
+  </si>
+  <si>
+    <t>0,944</t>
+  </si>
+  <si>
+    <t>0,943</t>
+  </si>
+  <si>
+    <t>0,935</t>
+  </si>
+  <si>
+    <t>0,921</t>
+  </si>
+  <si>
+    <t>0,969</t>
+  </si>
+  <si>
+    <t>0,761</t>
+  </si>
+  <si>
+    <t>0,723</t>
+  </si>
+  <si>
+    <t>0,714</t>
+  </si>
+  <si>
+    <t>0,015</t>
+  </si>
+  <si>
+    <t>0,970</t>
+  </si>
+  <si>
+    <t>0,906</t>
+  </si>
+  <si>
+    <t>0,872</t>
+  </si>
+  <si>
+    <t>0,861</t>
+  </si>
+  <si>
+    <t>0,852</t>
+  </si>
+  <si>
+    <t>Transcription factor inhibito</t>
+  </si>
+  <si>
+    <t>0,988</t>
+  </si>
+  <si>
+    <t>0,927</t>
+  </si>
+  <si>
+    <t>0,874</t>
+  </si>
+  <si>
+    <t>0,835</t>
+  </si>
+  <si>
+    <t>0,808</t>
+  </si>
+  <si>
+    <t>0,960</t>
+  </si>
+  <si>
+    <t>0,746</t>
+  </si>
+  <si>
+    <t>0,011</t>
+  </si>
+  <si>
+    <t>0,702</t>
+  </si>
+  <si>
+    <t>0,986</t>
+  </si>
+  <si>
+    <t>0,976</t>
+  </si>
+  <si>
+    <t>0,973</t>
+  </si>
+  <si>
+    <t>0,917</t>
+  </si>
+  <si>
+    <t>0,880</t>
+  </si>
+  <si>
+    <t>0,863</t>
+  </si>
+  <si>
+    <t>0,817</t>
+  </si>
+  <si>
+    <t>0,990</t>
+  </si>
+  <si>
+    <t>0,985</t>
+  </si>
+  <si>
+    <t>0,974</t>
+  </si>
+  <si>
+    <t>0,938</t>
+  </si>
+  <si>
+    <t>0,855</t>
+  </si>
+  <si>
+    <t>0,842</t>
+  </si>
+  <si>
+    <t>0,815</t>
+  </si>
+  <si>
+    <t>0,993</t>
+  </si>
+  <si>
+    <t>0,936</t>
+  </si>
+  <si>
+    <t>0,889</t>
+  </si>
+  <si>
+    <t>0,862</t>
+  </si>
+  <si>
+    <t>0,964</t>
+  </si>
+  <si>
+    <t>0,967</t>
+  </si>
+  <si>
+    <t>0,963</t>
+  </si>
+  <si>
+    <t>0,942</t>
+  </si>
+  <si>
+    <t>0,854</t>
+  </si>
+  <si>
+    <t>0,836</t>
+  </si>
+  <si>
+    <t>0,946</t>
+  </si>
+  <si>
+    <t>0,859</t>
+  </si>
+  <si>
+    <t>0,856</t>
+  </si>
+  <si>
+    <t>0,826</t>
+  </si>
+  <si>
+    <t>0,884</t>
+  </si>
+  <si>
+    <t>0,992</t>
+  </si>
+  <si>
+    <t>0,987</t>
+  </si>
+  <si>
+    <t>0,920</t>
+  </si>
+  <si>
+    <t>0,873</t>
+  </si>
+  <si>
+    <t>0,840</t>
+  </si>
+  <si>
+    <t>0,981</t>
+  </si>
+  <si>
+    <t>0,901</t>
+  </si>
+  <si>
+    <t>0,875</t>
+  </si>
+  <si>
+    <t>0,860</t>
+  </si>
+  <si>
+    <t>0,822</t>
+  </si>
+  <si>
+    <t>0,972</t>
+  </si>
+  <si>
+    <t>0,925</t>
+  </si>
+  <si>
+    <t>0,908</t>
+  </si>
+  <si>
+    <t>0,814</t>
+  </si>
+  <si>
+    <t>0,784</t>
+  </si>
+  <si>
+    <t>0,991</t>
+  </si>
+  <si>
+    <t>0,965</t>
+  </si>
+  <si>
+    <t>0,931</t>
+  </si>
+  <si>
+    <t>0,871</t>
+  </si>
+  <si>
+    <t>0,012</t>
+  </si>
+  <si>
+    <t>0,802</t>
+  </si>
+  <si>
+    <t>0,710</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2354,12 +2755,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2381,7 +2776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2399,12 +2794,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2688,8 +3077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12356,7 +12745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JS25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
+    <sheetView topLeftCell="CA1" workbookViewId="0">
       <selection activeCell="CB1" sqref="CB1"/>
     </sheetView>
   </sheetViews>
@@ -32970,10 +33359,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A101"/>
+  <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H101"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177:A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32981,308 +33370,2599 @@
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="5"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="5"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="5"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="5"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="5"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="5"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="5"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="5"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="5"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="5"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="5"/>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>720</v>
+      </c>
+      <c r="C1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>714</v>
+      </c>
+      <c r="C2" t="s">
+        <v>715</v>
+      </c>
+      <c r="D2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>717</v>
+      </c>
+      <c r="C3" t="s">
+        <v>718</v>
+      </c>
+      <c r="D3" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>723</v>
+      </c>
+      <c r="C4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D4" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>725</v>
+      </c>
+      <c r="C5" t="s">
+        <v>715</v>
+      </c>
+      <c r="D5" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>727</v>
+      </c>
+      <c r="C6" t="s">
+        <v>715</v>
+      </c>
+      <c r="D6" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>729</v>
+      </c>
+      <c r="C7" t="s">
+        <v>730</v>
+      </c>
+      <c r="D7" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>732</v>
+      </c>
+      <c r="C8" t="s">
+        <v>733</v>
+      </c>
+      <c r="D8" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>735</v>
+      </c>
+      <c r="C9" t="s">
+        <v>724</v>
+      </c>
+      <c r="D9" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>736</v>
+      </c>
+      <c r="C10" t="s">
+        <v>737</v>
+      </c>
+      <c r="D10" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>738</v>
+      </c>
+      <c r="C11" t="s">
+        <v>718</v>
+      </c>
+      <c r="D11" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>729</v>
+      </c>
+      <c r="C12" t="s">
+        <v>730</v>
+      </c>
+      <c r="D12" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>739</v>
+      </c>
+      <c r="C13" t="s">
+        <v>724</v>
+      </c>
+      <c r="D13" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>740</v>
+      </c>
+      <c r="C14" t="s">
+        <v>741</v>
+      </c>
+      <c r="D14" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>743</v>
+      </c>
+      <c r="C15" t="s">
+        <v>744</v>
+      </c>
+      <c r="D15" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>745</v>
+      </c>
+      <c r="C16" t="s">
+        <v>724</v>
+      </c>
+      <c r="D16" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>746</v>
+      </c>
+      <c r="C17" t="s">
+        <v>747</v>
+      </c>
+      <c r="D17" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>749</v>
+      </c>
+      <c r="C18" t="s">
+        <v>750</v>
+      </c>
+      <c r="D18" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>752</v>
+      </c>
+      <c r="C19" t="s">
+        <v>753</v>
+      </c>
+      <c r="D19" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>755</v>
+      </c>
+      <c r="C20" t="s">
+        <v>724</v>
+      </c>
+      <c r="D20" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>756</v>
+      </c>
+      <c r="C21" t="s">
+        <v>747</v>
+      </c>
+      <c r="D21" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>758</v>
+      </c>
+      <c r="C22" t="s">
+        <v>759</v>
+      </c>
+      <c r="D22" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>760</v>
+      </c>
+      <c r="C23" t="s">
+        <v>747</v>
+      </c>
+      <c r="D23" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>762</v>
+      </c>
+      <c r="C24" t="s">
+        <v>747</v>
+      </c>
+      <c r="D24" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>764</v>
+      </c>
+      <c r="C25" t="s">
+        <v>747</v>
+      </c>
+      <c r="D25" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>766</v>
+      </c>
+      <c r="C26" t="s">
+        <v>724</v>
+      </c>
+      <c r="D26" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>767</v>
+      </c>
+      <c r="C27" t="s">
+        <v>741</v>
+      </c>
+      <c r="D27" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>768</v>
+      </c>
+      <c r="C28" t="s">
+        <v>747</v>
+      </c>
+      <c r="D28" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>770</v>
+      </c>
+      <c r="C29" t="s">
+        <v>771</v>
+      </c>
+      <c r="D29" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>773</v>
+      </c>
+      <c r="C30" t="s">
+        <v>774</v>
+      </c>
+      <c r="D30" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>775</v>
+      </c>
+      <c r="C31" t="s">
+        <v>776</v>
+      </c>
+      <c r="D31" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>777</v>
+      </c>
+      <c r="C32" t="s">
+        <v>724</v>
+      </c>
+      <c r="D32" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>778</v>
+      </c>
+      <c r="C33" t="s">
+        <v>747</v>
+      </c>
+      <c r="D33" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>779</v>
+      </c>
+      <c r="C34" t="s">
+        <v>741</v>
+      </c>
+      <c r="D34" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>779</v>
+      </c>
+      <c r="C35" t="s">
+        <v>771</v>
+      </c>
+      <c r="D35" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>781</v>
+      </c>
+      <c r="C36" t="s">
+        <v>741</v>
+      </c>
+      <c r="D36" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
+        <v>782</v>
+      </c>
+      <c r="C37" t="s">
+        <v>747</v>
+      </c>
+      <c r="D37" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>783</v>
+      </c>
+      <c r="C38" t="s">
+        <v>776</v>
+      </c>
+      <c r="D38" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>785</v>
+      </c>
+      <c r="C39" t="s">
+        <v>786</v>
+      </c>
+      <c r="D39" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>755</v>
+      </c>
+      <c r="C40" t="s">
+        <v>741</v>
+      </c>
+      <c r="D40" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>787</v>
+      </c>
+      <c r="C41" t="s">
+        <v>724</v>
+      </c>
+      <c r="D41" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>777</v>
+      </c>
+      <c r="C42" t="s">
+        <v>771</v>
+      </c>
+      <c r="D42" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>788</v>
+      </c>
+      <c r="C43" t="s">
+        <v>759</v>
+      </c>
+      <c r="D43" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>789</v>
+      </c>
+      <c r="C44" t="s">
+        <v>724</v>
+      </c>
+      <c r="D44" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" t="s">
+        <v>783</v>
+      </c>
+      <c r="C45" t="s">
+        <v>776</v>
+      </c>
+      <c r="D45" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>790</v>
+      </c>
+      <c r="C46" t="s">
+        <v>771</v>
+      </c>
+      <c r="D46" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>791</v>
+      </c>
+      <c r="C47" t="s">
+        <v>741</v>
+      </c>
+      <c r="D47" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>758</v>
+      </c>
+      <c r="C48" t="s">
+        <v>724</v>
+      </c>
+      <c r="D48" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>792</v>
+      </c>
+      <c r="C49" t="s">
+        <v>771</v>
+      </c>
+      <c r="D49" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B50" t="s">
+        <v>793</v>
+      </c>
+      <c r="C50" t="s">
+        <v>747</v>
+      </c>
+      <c r="D50" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
+        <v>794</v>
+      </c>
+      <c r="C51" t="s">
+        <v>741</v>
+      </c>
+      <c r="D51" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" t="s">
+        <v>795</v>
+      </c>
+      <c r="C52" t="s">
+        <v>747</v>
+      </c>
+      <c r="D52" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" t="s">
+        <v>764</v>
+      </c>
+      <c r="C53" t="s">
+        <v>741</v>
+      </c>
+      <c r="D53" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>796</v>
+      </c>
+      <c r="C54" t="s">
+        <v>724</v>
+      </c>
+      <c r="D54" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>745</v>
+      </c>
+      <c r="C55" t="s">
+        <v>724</v>
+      </c>
+      <c r="D55" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>797</v>
+      </c>
+      <c r="C56" t="s">
+        <v>747</v>
+      </c>
+      <c r="D56" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
+        <v>798</v>
+      </c>
+      <c r="C57" t="s">
+        <v>718</v>
+      </c>
+      <c r="D57" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>799</v>
+      </c>
+      <c r="C58" t="s">
+        <v>800</v>
+      </c>
+      <c r="D58" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
+        <v>756</v>
+      </c>
+      <c r="C59" t="s">
+        <v>724</v>
+      </c>
+      <c r="D59" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>29</v>
+      </c>
+      <c r="B60" t="s">
+        <v>801</v>
+      </c>
+      <c r="C60" t="s">
+        <v>771</v>
+      </c>
+      <c r="D60" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" t="s">
+        <v>778</v>
+      </c>
+      <c r="C61" t="s">
+        <v>759</v>
+      </c>
+      <c r="D61" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>29</v>
+      </c>
+      <c r="B62" t="s">
+        <v>802</v>
+      </c>
+      <c r="C62" t="s">
+        <v>771</v>
+      </c>
+      <c r="D62" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" t="s">
+        <v>803</v>
+      </c>
+      <c r="C63" t="s">
+        <v>715</v>
+      </c>
+      <c r="D63" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>804</v>
+      </c>
+      <c r="C64" t="s">
+        <v>747</v>
+      </c>
+      <c r="D64" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>805</v>
+      </c>
+      <c r="C65" t="s">
+        <v>747</v>
+      </c>
+      <c r="D65" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" t="s">
+        <v>807</v>
+      </c>
+      <c r="C66" t="s">
+        <v>724</v>
+      </c>
+      <c r="D66" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" t="s">
+        <v>787</v>
+      </c>
+      <c r="C67" t="s">
+        <v>747</v>
+      </c>
+      <c r="D67" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" t="s">
+        <v>801</v>
+      </c>
+      <c r="C68" t="s">
+        <v>759</v>
+      </c>
+      <c r="D68" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>808</v>
+      </c>
+      <c r="C69" t="s">
+        <v>771</v>
+      </c>
+      <c r="D69" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" t="s">
+        <v>809</v>
+      </c>
+      <c r="C70" t="s">
+        <v>747</v>
+      </c>
+      <c r="D70" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" t="s">
+        <v>783</v>
+      </c>
+      <c r="C71" t="s">
+        <v>715</v>
+      </c>
+      <c r="D71" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" t="s">
+        <v>767</v>
+      </c>
+      <c r="C72" t="s">
+        <v>741</v>
+      </c>
+      <c r="D72" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" t="s">
+        <v>810</v>
+      </c>
+      <c r="C73" t="s">
+        <v>741</v>
+      </c>
+      <c r="D73" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" t="s">
+        <v>811</v>
+      </c>
+      <c r="C74" t="s">
+        <v>771</v>
+      </c>
+      <c r="D74" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75" t="s">
+        <v>812</v>
+      </c>
+      <c r="C75" t="s">
+        <v>724</v>
+      </c>
+      <c r="D75" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76" t="s">
+        <v>736</v>
+      </c>
+      <c r="C76" t="s">
+        <v>737</v>
+      </c>
+      <c r="D76" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" t="s">
+        <v>813</v>
+      </c>
+      <c r="C77" t="s">
+        <v>814</v>
+      </c>
+      <c r="D77" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" t="s">
+        <v>738</v>
+      </c>
+      <c r="C78" t="s">
+        <v>718</v>
+      </c>
+      <c r="D78" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79" t="s">
+        <v>815</v>
+      </c>
+      <c r="C79" t="s">
+        <v>715</v>
+      </c>
+      <c r="D79" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" t="s">
+        <v>816</v>
+      </c>
+      <c r="C80" t="s">
+        <v>724</v>
+      </c>
+      <c r="D80" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" t="s">
+        <v>758</v>
+      </c>
+      <c r="C81" t="s">
+        <v>747</v>
+      </c>
+      <c r="D81" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>34</v>
+      </c>
+      <c r="B82" t="s">
+        <v>817</v>
+      </c>
+      <c r="C82" t="s">
+        <v>747</v>
+      </c>
+      <c r="D82" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" t="s">
+        <v>818</v>
+      </c>
+      <c r="C83" t="s">
+        <v>759</v>
+      </c>
+      <c r="D83" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B84" t="s">
+        <v>819</v>
+      </c>
+      <c r="C84" t="s">
+        <v>724</v>
+      </c>
+      <c r="D84" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" t="s">
+        <v>820</v>
+      </c>
+      <c r="C85" t="s">
+        <v>747</v>
+      </c>
+      <c r="D85" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>34</v>
+      </c>
+      <c r="B86" t="s">
+        <v>821</v>
+      </c>
+      <c r="C86" t="s">
+        <v>741</v>
+      </c>
+      <c r="D86" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>34</v>
+      </c>
+      <c r="B87" t="s">
+        <v>822</v>
+      </c>
+      <c r="C87" t="s">
+        <v>771</v>
+      </c>
+      <c r="D87" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>823</v>
+      </c>
+      <c r="C88" t="s">
+        <v>771</v>
+      </c>
+      <c r="D88" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>824</v>
+      </c>
+      <c r="C89" t="s">
+        <v>747</v>
+      </c>
+      <c r="D89" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>825</v>
+      </c>
+      <c r="C90" t="s">
+        <v>759</v>
+      </c>
+      <c r="D90" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" t="s">
+        <v>826</v>
+      </c>
+      <c r="C91" t="s">
+        <v>747</v>
+      </c>
+      <c r="D91" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" t="s">
+        <v>735</v>
+      </c>
+      <c r="C92" t="s">
+        <v>724</v>
+      </c>
+      <c r="D92" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93" t="s">
+        <v>827</v>
+      </c>
+      <c r="C93" t="s">
+        <v>741</v>
+      </c>
+      <c r="D93" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" t="s">
+        <v>828</v>
+      </c>
+      <c r="C94" t="s">
+        <v>747</v>
+      </c>
+      <c r="D94" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>28</v>
+      </c>
+      <c r="B95" t="s">
+        <v>829</v>
+      </c>
+      <c r="C95" t="s">
+        <v>771</v>
+      </c>
+      <c r="D95" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B96" t="s">
+        <v>830</v>
+      </c>
+      <c r="C96" t="s">
+        <v>771</v>
+      </c>
+      <c r="D96" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B97" t="s">
+        <v>816</v>
+      </c>
+      <c r="C97" t="s">
+        <v>747</v>
+      </c>
+      <c r="D97" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>31</v>
+      </c>
+      <c r="B98" t="s">
+        <v>787</v>
+      </c>
+      <c r="C98" t="s">
+        <v>759</v>
+      </c>
+      <c r="D98" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>31</v>
+      </c>
+      <c r="B99" t="s">
+        <v>778</v>
+      </c>
+      <c r="C99" t="s">
+        <v>747</v>
+      </c>
+      <c r="D99" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100" t="s">
+        <v>831</v>
+      </c>
+      <c r="C100" t="s">
+        <v>724</v>
+      </c>
+      <c r="D100" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>31</v>
+      </c>
+      <c r="B101" t="s">
+        <v>832</v>
+      </c>
+      <c r="C101" t="s">
+        <v>747</v>
+      </c>
+      <c r="D101" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>31</v>
+      </c>
+      <c r="B102" t="s">
+        <v>833</v>
+      </c>
+      <c r="C102" t="s">
+        <v>747</v>
+      </c>
+      <c r="D102" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>31</v>
+      </c>
+      <c r="B103" t="s">
+        <v>805</v>
+      </c>
+      <c r="C103" t="s">
+        <v>741</v>
+      </c>
+      <c r="D103" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" t="s">
+        <v>810</v>
+      </c>
+      <c r="C104" t="s">
+        <v>747</v>
+      </c>
+      <c r="D104" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>33</v>
+      </c>
+      <c r="B105" t="s">
+        <v>834</v>
+      </c>
+      <c r="C105" t="s">
+        <v>759</v>
+      </c>
+      <c r="D105" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B106" t="s">
+        <v>835</v>
+      </c>
+      <c r="C106" t="s">
+        <v>724</v>
+      </c>
+      <c r="D106" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>33</v>
+      </c>
+      <c r="B107" t="s">
+        <v>836</v>
+      </c>
+      <c r="C107" t="s">
+        <v>771</v>
+      </c>
+      <c r="D107" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>33</v>
+      </c>
+      <c r="B108" t="s">
+        <v>837</v>
+      </c>
+      <c r="C108" t="s">
+        <v>747</v>
+      </c>
+      <c r="D108" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>33</v>
+      </c>
+      <c r="B109" t="s">
+        <v>833</v>
+      </c>
+      <c r="C109" t="s">
+        <v>715</v>
+      </c>
+      <c r="D109" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B110" t="s">
+        <v>838</v>
+      </c>
+      <c r="C110" t="s">
+        <v>741</v>
+      </c>
+      <c r="D110" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>33</v>
+      </c>
+      <c r="B111" t="s">
+        <v>839</v>
+      </c>
+      <c r="C111" t="s">
+        <v>747</v>
+      </c>
+      <c r="D111" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" t="s">
+        <v>787</v>
+      </c>
+      <c r="C112" t="s">
+        <v>759</v>
+      </c>
+      <c r="D112" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" t="s">
+        <v>818</v>
+      </c>
+      <c r="C113" t="s">
+        <v>771</v>
+      </c>
+      <c r="D113" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" t="s">
+        <v>801</v>
+      </c>
+      <c r="C114" t="s">
+        <v>724</v>
+      </c>
+      <c r="D114" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" t="s">
+        <v>840</v>
+      </c>
+      <c r="C115" t="s">
+        <v>747</v>
+      </c>
+      <c r="D115" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" t="s">
+        <v>766</v>
+      </c>
+      <c r="C116" t="s">
+        <v>724</v>
+      </c>
+      <c r="D116" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" t="s">
+        <v>841</v>
+      </c>
+      <c r="C117" t="s">
+        <v>747</v>
+      </c>
+      <c r="D117" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" t="s">
+        <v>842</v>
+      </c>
+      <c r="C118" t="s">
+        <v>741</v>
+      </c>
+      <c r="D118" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" t="s">
+        <v>785</v>
+      </c>
+      <c r="C119" t="s">
+        <v>747</v>
+      </c>
+      <c r="D119" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" t="s">
+        <v>843</v>
+      </c>
+      <c r="C120" t="s">
+        <v>771</v>
+      </c>
+      <c r="D120" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>37</v>
+      </c>
+      <c r="B121" t="s">
+        <v>835</v>
+      </c>
+      <c r="C121" t="s">
+        <v>724</v>
+      </c>
+      <c r="D121" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>37</v>
+      </c>
+      <c r="B122" t="s">
+        <v>812</v>
+      </c>
+      <c r="C122" t="s">
+        <v>771</v>
+      </c>
+      <c r="D122" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>37</v>
+      </c>
+      <c r="B123" t="s">
+        <v>840</v>
+      </c>
+      <c r="C123" t="s">
+        <v>741</v>
+      </c>
+      <c r="D123" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>37</v>
+      </c>
+      <c r="B124" t="s">
+        <v>844</v>
+      </c>
+      <c r="C124" t="s">
+        <v>715</v>
+      </c>
+      <c r="D124" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>656</v>
+      </c>
+      <c r="B125" t="s">
+        <v>845</v>
+      </c>
+      <c r="C125" t="s">
+        <v>771</v>
+      </c>
+      <c r="D125" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>656</v>
+      </c>
+      <c r="B126" t="s">
+        <v>846</v>
+      </c>
+      <c r="C126" t="s">
+        <v>747</v>
+      </c>
+      <c r="D126" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>656</v>
+      </c>
+      <c r="B127" t="s">
+        <v>787</v>
+      </c>
+      <c r="C127" t="s">
+        <v>759</v>
+      </c>
+      <c r="D127" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>656</v>
+      </c>
+      <c r="B128" t="s">
+        <v>808</v>
+      </c>
+      <c r="C128" t="s">
+        <v>747</v>
+      </c>
+      <c r="D128" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>656</v>
+      </c>
+      <c r="B129" t="s">
+        <v>847</v>
+      </c>
+      <c r="C129" t="s">
+        <v>747</v>
+      </c>
+      <c r="D129" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>656</v>
+      </c>
+      <c r="B130" t="s">
+        <v>714</v>
+      </c>
+      <c r="C130" t="s">
+        <v>724</v>
+      </c>
+      <c r="D130" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>656</v>
+      </c>
+      <c r="B131" t="s">
+        <v>848</v>
+      </c>
+      <c r="C131" t="s">
+        <v>741</v>
+      </c>
+      <c r="D131" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>656</v>
+      </c>
+      <c r="B132" t="s">
+        <v>849</v>
+      </c>
+      <c r="C132" t="s">
+        <v>747</v>
+      </c>
+      <c r="D132" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>665</v>
+      </c>
+      <c r="B133" t="s">
+        <v>823</v>
+      </c>
+      <c r="C133" t="s">
+        <v>771</v>
+      </c>
+      <c r="D133" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>665</v>
+      </c>
+      <c r="B134" t="s">
+        <v>850</v>
+      </c>
+      <c r="C134" t="s">
+        <v>747</v>
+      </c>
+      <c r="D134" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>665</v>
+      </c>
+      <c r="B135" t="s">
+        <v>850</v>
+      </c>
+      <c r="C135" t="s">
+        <v>747</v>
+      </c>
+      <c r="D135" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>665</v>
+      </c>
+      <c r="B136" t="s">
+        <v>825</v>
+      </c>
+      <c r="C136" t="s">
+        <v>759</v>
+      </c>
+      <c r="D136" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>665</v>
+      </c>
+      <c r="B137" t="s">
+        <v>762</v>
+      </c>
+      <c r="C137" t="s">
+        <v>724</v>
+      </c>
+      <c r="D137" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>665</v>
+      </c>
+      <c r="B138" t="s">
+        <v>851</v>
+      </c>
+      <c r="C138" t="s">
+        <v>747</v>
+      </c>
+      <c r="D138" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>665</v>
+      </c>
+      <c r="B139" t="s">
+        <v>852</v>
+      </c>
+      <c r="C139" t="s">
+        <v>741</v>
+      </c>
+      <c r="D139" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>665</v>
+      </c>
+      <c r="B140" t="s">
+        <v>853</v>
+      </c>
+      <c r="C140" t="s">
+        <v>747</v>
+      </c>
+      <c r="D140" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>665</v>
+      </c>
+      <c r="B141" t="s">
+        <v>854</v>
+      </c>
+      <c r="C141" t="s">
+        <v>771</v>
+      </c>
+      <c r="D141" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>665</v>
+      </c>
+      <c r="B142" t="s">
+        <v>823</v>
+      </c>
+      <c r="C142" t="s">
+        <v>771</v>
+      </c>
+      <c r="D142" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>665</v>
+      </c>
+      <c r="B143" t="s">
+        <v>850</v>
+      </c>
+      <c r="C143" t="s">
+        <v>747</v>
+      </c>
+      <c r="D143" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>665</v>
+      </c>
+      <c r="B144" t="s">
+        <v>850</v>
+      </c>
+      <c r="C144" t="s">
+        <v>747</v>
+      </c>
+      <c r="D144" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>665</v>
+      </c>
+      <c r="B145" t="s">
+        <v>825</v>
+      </c>
+      <c r="C145" t="s">
+        <v>759</v>
+      </c>
+      <c r="D145" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>665</v>
+      </c>
+      <c r="B146" t="s">
+        <v>762</v>
+      </c>
+      <c r="C146" t="s">
+        <v>724</v>
+      </c>
+      <c r="D146" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>665</v>
+      </c>
+      <c r="B147" t="s">
+        <v>851</v>
+      </c>
+      <c r="C147" t="s">
+        <v>747</v>
+      </c>
+      <c r="D147" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>665</v>
+      </c>
+      <c r="B148" t="s">
+        <v>852</v>
+      </c>
+      <c r="C148" t="s">
+        <v>741</v>
+      </c>
+      <c r="D148" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>665</v>
+      </c>
+      <c r="B149" t="s">
+        <v>853</v>
+      </c>
+      <c r="C149" t="s">
+        <v>747</v>
+      </c>
+      <c r="D149" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>665</v>
+      </c>
+      <c r="B150" t="s">
+        <v>854</v>
+      </c>
+      <c r="C150" t="s">
+        <v>771</v>
+      </c>
+      <c r="D150" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>666</v>
+      </c>
+      <c r="B151" t="s">
+        <v>823</v>
+      </c>
+      <c r="C151" t="s">
+        <v>771</v>
+      </c>
+      <c r="D151" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>666</v>
+      </c>
+      <c r="B152" t="s">
+        <v>855</v>
+      </c>
+      <c r="C152" t="s">
+        <v>771</v>
+      </c>
+      <c r="D152" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>666</v>
+      </c>
+      <c r="B153" t="s">
+        <v>777</v>
+      </c>
+      <c r="C153" t="s">
+        <v>759</v>
+      </c>
+      <c r="D153" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>666</v>
+      </c>
+      <c r="B154" t="s">
+        <v>856</v>
+      </c>
+      <c r="C154" t="s">
+        <v>771</v>
+      </c>
+      <c r="D154" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>666</v>
+      </c>
+      <c r="B155" t="s">
+        <v>857</v>
+      </c>
+      <c r="C155" t="s">
+        <v>724</v>
+      </c>
+      <c r="D155" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>666</v>
+      </c>
+      <c r="B156" t="s">
+        <v>821</v>
+      </c>
+      <c r="C156" t="s">
+        <v>741</v>
+      </c>
+      <c r="D156" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>666</v>
+      </c>
+      <c r="B157" t="s">
+        <v>858</v>
+      </c>
+      <c r="C157" t="s">
+        <v>771</v>
+      </c>
+      <c r="D157" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>660</v>
+      </c>
+      <c r="B158" t="s">
+        <v>830</v>
+      </c>
+      <c r="C158" t="s">
+        <v>771</v>
+      </c>
+      <c r="D158" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>660</v>
+      </c>
+      <c r="B159" t="s">
+        <v>816</v>
+      </c>
+      <c r="C159" t="s">
+        <v>747</v>
+      </c>
+      <c r="D159" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>660</v>
+      </c>
+      <c r="B160" t="s">
+        <v>787</v>
+      </c>
+      <c r="C160" t="s">
+        <v>759</v>
+      </c>
+      <c r="D160" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>660</v>
+      </c>
+      <c r="B161" t="s">
+        <v>778</v>
+      </c>
+      <c r="C161" t="s">
+        <v>747</v>
+      </c>
+      <c r="D161" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>660</v>
+      </c>
+      <c r="B162" t="s">
+        <v>831</v>
+      </c>
+      <c r="C162" t="s">
+        <v>724</v>
+      </c>
+      <c r="D162" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>660</v>
+      </c>
+      <c r="B163" t="s">
+        <v>832</v>
+      </c>
+      <c r="C163" t="s">
+        <v>747</v>
+      </c>
+      <c r="D163" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>660</v>
+      </c>
+      <c r="B164" t="s">
+        <v>833</v>
+      </c>
+      <c r="C164" t="s">
+        <v>747</v>
+      </c>
+      <c r="D164" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>660</v>
+      </c>
+      <c r="B165" t="s">
+        <v>805</v>
+      </c>
+      <c r="C165" t="s">
+        <v>741</v>
+      </c>
+      <c r="D165" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>660</v>
+      </c>
+      <c r="B166" t="s">
+        <v>810</v>
+      </c>
+      <c r="C166" t="s">
+        <v>747</v>
+      </c>
+      <c r="D166" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>662</v>
+      </c>
+      <c r="B167" t="s">
+        <v>830</v>
+      </c>
+      <c r="C167" t="s">
+        <v>771</v>
+      </c>
+      <c r="D167" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>662</v>
+      </c>
+      <c r="B168" t="s">
+        <v>816</v>
+      </c>
+      <c r="C168" t="s">
+        <v>747</v>
+      </c>
+      <c r="D168" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>662</v>
+      </c>
+      <c r="B169" t="s">
+        <v>787</v>
+      </c>
+      <c r="C169" t="s">
+        <v>759</v>
+      </c>
+      <c r="D169" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>662</v>
+      </c>
+      <c r="B170" t="s">
+        <v>778</v>
+      </c>
+      <c r="C170" t="s">
+        <v>747</v>
+      </c>
+      <c r="D170" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>662</v>
+      </c>
+      <c r="B171" t="s">
+        <v>831</v>
+      </c>
+      <c r="C171" t="s">
+        <v>724</v>
+      </c>
+      <c r="D171" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>662</v>
+      </c>
+      <c r="B172" t="s">
+        <v>832</v>
+      </c>
+      <c r="C172" t="s">
+        <v>747</v>
+      </c>
+      <c r="D172" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>662</v>
+      </c>
+      <c r="B173" t="s">
+        <v>833</v>
+      </c>
+      <c r="C173" t="s">
+        <v>747</v>
+      </c>
+      <c r="D173" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>662</v>
+      </c>
+      <c r="B174" t="s">
+        <v>805</v>
+      </c>
+      <c r="C174" t="s">
+        <v>741</v>
+      </c>
+      <c r="D174" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>662</v>
+      </c>
+      <c r="B175" t="s">
+        <v>810</v>
+      </c>
+      <c r="C175" t="s">
+        <v>747</v>
+      </c>
+      <c r="D175" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>662</v>
+      </c>
+      <c r="B176" t="s">
+        <v>859</v>
+      </c>
+      <c r="C176" t="s">
+        <v>771</v>
+      </c>
+      <c r="D176" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>667</v>
+      </c>
+      <c r="B177" t="s">
+        <v>860</v>
+      </c>
+      <c r="C177" t="s">
+        <v>771</v>
+      </c>
+      <c r="D177" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>667</v>
+      </c>
+      <c r="B178" t="s">
+        <v>818</v>
+      </c>
+      <c r="C178" t="s">
+        <v>771</v>
+      </c>
+      <c r="D178" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>667</v>
+      </c>
+      <c r="B179" t="s">
+        <v>861</v>
+      </c>
+      <c r="C179" t="s">
+        <v>759</v>
+      </c>
+      <c r="D179" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>667</v>
+      </c>
+      <c r="B180" t="s">
+        <v>862</v>
+      </c>
+      <c r="C180" t="s">
+        <v>724</v>
+      </c>
+      <c r="D180" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>667</v>
+      </c>
+      <c r="B181" t="s">
+        <v>863</v>
+      </c>
+      <c r="C181" t="s">
+        <v>724</v>
+      </c>
+      <c r="D181" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>667</v>
+      </c>
+      <c r="B182" t="s">
+        <v>810</v>
+      </c>
+      <c r="C182" t="s">
+        <v>741</v>
+      </c>
+      <c r="D182" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>667</v>
+      </c>
+      <c r="B183" t="s">
+        <v>785</v>
+      </c>
+      <c r="C183" t="s">
+        <v>864</v>
+      </c>
+      <c r="D183" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>667</v>
+      </c>
+      <c r="B184" t="s">
+        <v>865</v>
+      </c>
+      <c r="C184" t="s">
+        <v>771</v>
+      </c>
+      <c r="D184" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>667</v>
+      </c>
+      <c r="B185" t="s">
+        <v>866</v>
+      </c>
+      <c r="C185" t="s">
+        <v>724</v>
+      </c>
+      <c r="D185" t="s">
+        <v>772</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33425,350 +36105,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>719</v>
-      </c>
-      <c r="B3" t="s">
-        <v>720</v>
-      </c>
-      <c r="C3" t="s">
-        <v>721</v>
-      </c>
-      <c r="D3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>718</v>
-      </c>
-      <c r="B4">
-        <v>0.13239999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>722</v>
-      </c>
-      <c r="B5">
-        <v>7.1999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>723</v>
-      </c>
-      <c r="B6" t="s">
-        <v>724</v>
-      </c>
-      <c r="C6">
-        <v>0.1376</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>725</v>
-      </c>
-      <c r="B7">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>726</v>
-      </c>
-      <c r="B8" t="s">
-        <v>727</v>
-      </c>
-      <c r="C8">
-        <v>5.3199999999999997E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>728</v>
-      </c>
-      <c r="B9" t="s">
-        <v>727</v>
-      </c>
-      <c r="C9">
-        <v>0.19750000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="B10">
-        <v>0.46100000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>730</v>
-      </c>
-      <c r="B11">
-        <v>0.14430000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>731</v>
-      </c>
-      <c r="B12" t="s">
-        <v>732</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>719</v>
-      </c>
-      <c r="B16" t="s">
-        <v>720</v>
-      </c>
-      <c r="C16" t="s">
-        <v>721</v>
-      </c>
-      <c r="D16">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>718</v>
-      </c>
-      <c r="B17">
-        <v>4.3395999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>722</v>
-      </c>
-      <c r="B18">
-        <v>3.6349999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>723</v>
-      </c>
-      <c r="B19" t="s">
-        <v>724</v>
-      </c>
-      <c r="C19">
-        <v>2.7888999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>725</v>
-      </c>
-      <c r="B20">
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>726</v>
-      </c>
-      <c r="B21" t="s">
-        <v>727</v>
-      </c>
-      <c r="C21">
-        <v>2.57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>728</v>
-      </c>
-      <c r="B22" t="s">
-        <v>727</v>
-      </c>
-      <c r="C22">
-        <v>4.8525</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="B23">
-        <v>12.95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>730</v>
-      </c>
-      <c r="B24">
-        <v>2.2825000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>731</v>
-      </c>
-      <c r="B25" t="s">
-        <v>732</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>719</v>
-      </c>
-      <c r="B29" t="s">
-        <v>720</v>
-      </c>
-      <c r="C29" t="s">
-        <v>721</v>
-      </c>
-      <c r="D29">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>718</v>
-      </c>
-      <c r="B30">
-        <v>0.71260000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>722</v>
-      </c>
-      <c r="B31">
-        <v>0.75049999999999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>723</v>
-      </c>
-      <c r="B32" t="s">
-        <v>724</v>
-      </c>
-      <c r="C32">
-        <v>0.123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>725</v>
-      </c>
-      <c r="B33">
-        <v>0.32300000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>726</v>
-      </c>
-      <c r="B34" t="s">
-        <v>727</v>
-      </c>
-      <c r="C34">
-        <v>0.67979999999999996</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>728</v>
-      </c>
-      <c r="B35" t="s">
-        <v>727</v>
-      </c>
-      <c r="C35">
-        <v>0.78480000000000005</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="B36">
-        <v>0.84899999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>730</v>
-      </c>
-      <c r="B37">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>731</v>
-      </c>
-      <c r="B38" t="s">
-        <v>732</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>